<commit_message>
First setup for swaps
</commit_message>
<xml_diff>
--- a/notebooks/df_curves.xlsx
+++ b/notebooks/df_curves.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF16"/>
+  <dimension ref="A1:Q16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -487,51 +487,6 @@
       <c r="Q1" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="T1" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="U1" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="W1" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="X1" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="Y1" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="AA1" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB1" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="AC1" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="AD1" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="AE1" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="AF1" s="1" t="n">
-        <v>30</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -585,51 +540,6 @@
       <c r="Q2" t="n">
         <v>3.052458844639447</v>
       </c>
-      <c r="R2" t="n">
-        <v>3.062458844639447</v>
-      </c>
-      <c r="S2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="T2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="U2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="V2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="W2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="X2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>3.052458844639447</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -683,51 +593,6 @@
       <c r="Q3" t="n">
         <v>3.052458844639447</v>
       </c>
-      <c r="R3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="S3" t="n">
-        <v>3.062458844639447</v>
-      </c>
-      <c r="T3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="U3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="V3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="W3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="X3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AE3" t="n">
-        <v>3.052458844639447</v>
-      </c>
-      <c r="AF3" t="n">
-        <v>3.052458844639447</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -781,51 +646,6 @@
       <c r="Q4" t="n">
         <v>3.369500170900171</v>
       </c>
-      <c r="R4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="S4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="T4" t="n">
-        <v>3.379500170900171</v>
-      </c>
-      <c r="U4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="V4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="W4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="X4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>3.369500170900171</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>3.369500170900171</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -879,51 +699,6 @@
       <c r="Q5" t="n">
         <v>3.390190664829394</v>
       </c>
-      <c r="R5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="S5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="T5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="U5" t="n">
-        <v>3.400190664829394</v>
-      </c>
-      <c r="V5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="W5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="X5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>3.390190664829394</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>3.390190664829394</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -977,51 +752,6 @@
       <c r="Q6" t="n">
         <v>3.28275774536765</v>
       </c>
-      <c r="R6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="S6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="T6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="U6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="V6" t="n">
-        <v>3.29275774536765</v>
-      </c>
-      <c r="W6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="X6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>3.28275774536765</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>3.28275774536765</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1075,51 +805,6 @@
       <c r="Q7" t="n">
         <v>3.135074441751974</v>
       </c>
-      <c r="R7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="S7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="T7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="U7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="V7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="W7" t="n">
-        <v>3.145074441751974</v>
-      </c>
-      <c r="X7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>3.135074441751974</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>3.135074441751974</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1173,51 +858,6 @@
       <c r="Q8" t="n">
         <v>2.989884603275789</v>
       </c>
-      <c r="R8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="S8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="T8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="U8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="V8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="W8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="X8" t="n">
-        <v>2.999884603275789</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>2.989884603275789</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>2.989884603275789</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1271,51 +911,6 @@
       <c r="Q9" t="n">
         <v>2.766859347519071</v>
       </c>
-      <c r="R9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="S9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="T9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="U9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="V9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="W9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="X9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>2.77685934751907</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>2.766859347519071</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>2.766859347519071</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1369,51 +964,6 @@
       <c r="Q10" t="n">
         <v>2.58844372913808</v>
       </c>
-      <c r="R10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="S10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="T10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="U10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="V10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="W10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="X10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>2.598443729138079</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="AB10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="AC10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="AD10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="AE10" t="n">
-        <v>2.58844372913808</v>
-      </c>
-      <c r="AF10" t="n">
-        <v>2.58844372913808</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1467,51 +1017,6 @@
       <c r="Q11" t="n">
         <v>2.586636230698117</v>
       </c>
-      <c r="R11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="S11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="T11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="U11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="V11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="W11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="X11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="Y11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="Z11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>2.596636230698116</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>2.586636230698117</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>2.586636230698117</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1565,51 +1070,6 @@
       <c r="Q12" t="n">
         <v>2.63002616242272</v>
       </c>
-      <c r="R12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="S12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="T12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="U12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="V12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="W12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="X12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="Y12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>2.64002616242272</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>2.63002616242272</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>2.63002616242272</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1663,51 +1123,6 @@
       <c r="Q13" t="n">
         <v>2.712942347675672</v>
       </c>
-      <c r="R13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="S13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="T13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="U13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="V13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="W13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="X13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="AA13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="AB13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>2.722942347675672</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>2.712942347675672</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>2.712942347675672</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1761,51 +1176,6 @@
       <c r="Q14" t="n">
         <v>2.767047309801201</v>
       </c>
-      <c r="R14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="S14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="T14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="U14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="V14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="W14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="X14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="AD14" t="n">
-        <v>2.777047309801201</v>
-      </c>
-      <c r="AE14" t="n">
-        <v>2.767047309801201</v>
-      </c>
-      <c r="AF14" t="n">
-        <v>2.767047309801201</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1859,51 +1229,6 @@
       <c r="Q15" t="n">
         <v>2.715402966371979</v>
       </c>
-      <c r="R15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="S15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="T15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="U15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="V15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="W15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="X15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="AB15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="AC15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>2.715402966371979</v>
-      </c>
-      <c r="AE15" t="n">
-        <v>2.725402966371978</v>
-      </c>
-      <c r="AF15" t="n">
-        <v>2.715402966371979</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1956,51 +1281,6 @@
       </c>
       <c r="Q16" t="n">
         <v>2.163018420006821</v>
-      </c>
-      <c r="R16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="S16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="T16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="U16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="V16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="W16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="X16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>2.173018420006821</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>2.183018420006821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>